<commit_message>
partial refactoring of MilestoneData. not working yet
</commit_message>
<xml_diff>
--- a/tests/resources/diff_milestone_data_formats_master_1_2020.xlsx
+++ b/tests/resources/diff_milestone_data_formats_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -34,37 +34,37 @@
     <t xml:space="preserve">Apollo 13</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6</t>
+    <t xml:space="preserve">Approval MM6</t>
   </si>
   <si>
     <t xml:space="preserve">Gateway Review 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 LoD</t>
+    <t xml:space="preserve">Approval MM6 LoD</t>
   </si>
   <si>
     <t xml:space="preserve">(2) IPA Gate 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Version No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assurance MM6 Original Baseline</t>
+    <t xml:space="preserve">Approval MM6 Version No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval MM6 Original Baseline</t>
   </si>
   <si>
     <t xml:space="preserve">26/04/2027</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Forecast - Actual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assurance MM6 Status</t>
+    <t xml:space="preserve">Approval MM6 Forecast - Actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval MM6 Status</t>
   </si>
   <si>
     <t xml:space="preserve">Live</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurance MM6 Notes</t>
+    <t xml:space="preserve">Approval MM6 Notes</t>
   </si>
   <si>
     <t xml:space="preserve">indicative dates tbc</t>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">Re-baseline IPDC milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Re-baseline IPDC cost</t>
@@ -228,10 +231,10 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="36.17"/>
   </cols>
@@ -393,30 +396,39 @@
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>